<commit_message>
finalizing the api version 1
</commit_message>
<xml_diff>
--- a/Sprint 2 - BackEnd/Planejamento/Planejamento_semanal-2.xlsx
+++ b/Sprint 2 - BackEnd/Planejamento/Planejamento_semanal-2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\OneDrive\Área de Trabalho\Projeto Inova\Sprint 2 - BackEnd\Planejamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\OneDrive\Área de Trabalho\InovaVagas\Sprint 2 - BackEnd\Planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39306FE3-AC5F-4DC5-9DCB-05CD7F81A596}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EDB841-8B89-499C-8F1B-003C5F473B2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
   <si>
     <t>PLANEJAMENTO SEMANAL - CONTROLE CLASSROOM</t>
   </si>
@@ -136,7 +136,7 @@
     <t>Em Andamento</t>
   </si>
   <si>
-    <t>Continuar a API</t>
+    <t>Tivemos que melhorar o banco de dados</t>
   </si>
 </sst>
 </file>
@@ -362,6 +362,12 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -378,12 +384,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
@@ -607,58 +607,60 @@
   </sheetPr>
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="35.7109375" customWidth="1"/>
     <col min="13" max="13" width="25.5703125" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="18"/>
     </row>
     <row r="2" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -673,68 +675,68 @@
       <c r="T2" s="3"/>
     </row>
     <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17" t="s">
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="17" t="s">
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="16"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="18"/>
     </row>
     <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="18">
+      <c r="A4" s="20">
         <v>44081</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="18">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="20">
         <v>44082</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="18">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="20">
         <v>44083</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="18">
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="20">
         <v>44084</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="18">
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="20">
         <v>44085</v>
       </c>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="16"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="18"/>
     </row>
     <row r="5" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -829,15 +831,19 @@
       <c r="N6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="6"/>
+      <c r="O6" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="6"/>
+      <c r="S6" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="T6" s="3"/>
     </row>
     <row r="7" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
@@ -871,11 +877,19 @@
       <c r="N7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="6"/>
+      <c r="O7" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="6"/>
+      <c r="Q7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="T7" s="3"/>
     </row>
     <row r="8" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
@@ -903,11 +917,19 @@
       <c r="N8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="6"/>
+      <c r="O8" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="6"/>
+      <c r="Q8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="S8" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="T8" s="3"/>
     </row>
     <row r="9" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
@@ -925,7 +947,7 @@
       <c r="J9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L9" s="3"/>
@@ -935,7 +957,9 @@
       <c r="N9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="6"/>
+      <c r="O9" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -957,7 +981,7 @@
       <c r="J10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L10" s="3"/>
@@ -967,7 +991,9 @@
       <c r="N10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="6"/>
+      <c r="O10" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
@@ -989,17 +1015,21 @@
       <c r="J11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="M11" s="11" t="s">
         <v>33</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="6"/>
+      <c r="O11" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
@@ -1031,7 +1061,9 @@
       <c r="N12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O12" s="6"/>
+      <c r="O12" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>

</xml_diff>